<commit_message>
lectura escritura excel from java
lectura y escritura de un archivo  excel con macros
</commit_message>
<xml_diff>
--- a/src/main/resources/contentExcel/caso1.xlsx
+++ b/src/main/resources/contentExcel/caso1.xlsx
@@ -2,25 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UTA_CALTU\ProWebCALTU\ProyectoWeb\src\main\resources\contentExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20940" windowHeight="9450"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28,7 +27,7 @@
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -336,14 +335,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>